<commit_message>
update sock PIC default
0.4 -> 0.04
</commit_message>
<xml_diff>
--- a/tier-1-grouping/PIC default product weights.xlsx
+++ b/tier-1-grouping/PIC default product weights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isaac.hopwood/Documents/GitHub/isaac-at-worldly/tier-1-grouping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4033C4D1-0D7C-704C-A038-A3BDB1CDA6FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08C851E-8CB6-204D-B932-6768D637A23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35720" yWindow="4780" windowWidth="24040" windowHeight="12380" xr2:uid="{6194EA15-A1D3-A446-9174-5FFFBC73106D}"/>
+    <workbookView xWindow="5200" yWindow="3100" windowWidth="24040" windowHeight="12380" xr2:uid="{6194EA15-A1D3-A446-9174-5FFFBC73106D}"/>
   </bookViews>
   <sheets>
     <sheet name="PIC default product weights" sheetId="1" r:id="rId1"/>
@@ -958,10 +958,14 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1037,7 +1041,7 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>0.4</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>